<commit_message>
resolve error in data
</commit_message>
<xml_diff>
--- a/data/Firm24_lijst.xlsx
+++ b/data/Firm24_lijst.xlsx
@@ -28,7 +28,7 @@
     <t>Zijn alle partijen Nederlandse rechtspersonen of natuurlijke personen?*</t>
   </si>
   <si>
-    <t>Ja, Nederlandse partijen; Nee, buitenlandsepartijen</t>
+    <t>Ja, Nederlandse partijen; Nee, buitenlandse partijen</t>
   </si>
   <si>
     <t>Zijn alle betrokken partijen de Nederlandse taal machtig?*</t>
@@ -150,10 +150,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,28 +464,28 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="95.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="75.14785714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -493,7 +493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -501,7 +501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -509,13 +509,13 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -523,13 +523,13 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -537,7 +537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -545,7 +545,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -553,7 +553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -561,7 +561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -569,7 +569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -577,7 +577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -593,7 +593,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -601,7 +601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -609,7 +609,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -617,7 +617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>